<commit_message>
Basic functionality all done
</commit_message>
<xml_diff>
--- a/Project2/questionList.xlsx
+++ b/Project2/questionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\SWE\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF6407-0346-4866-8F92-FF6F58997560}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B703986-F270-40A5-93C4-14A373FB1F54}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{64A99886-B78F-41ED-9737-B3D4DCE76225}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Questions</t>
   </si>
@@ -38,15 +38,9 @@
     <t>Who are you?</t>
   </si>
   <si>
-    <t>Nick</t>
-  </si>
-  <si>
     <t>What is your favorite color?</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>What do you love?</t>
   </si>
   <si>
@@ -54,6 +48,27 @@
   </si>
   <si>
     <t>Answers</t>
+  </si>
+  <si>
+    <t>sadf?</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>who eat cats?</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>who farted?</t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>blue</t>
   </si>
 </sst>
 </file>
@@ -405,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3317B68-4709-46B3-9CC9-5FE51B2C2F71}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -426,23 +441,47 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>